<commit_message>
BOM changed and more information added
</commit_message>
<xml_diff>
--- a/BOM/TriMod Adapter 2.xlsx
+++ b/BOM/TriMod Adapter 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elektronik\Altium\Projects\TriMod Adapter 2\Project Outputs for TriMod Adapter 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\TriMod_2.0_Adapter\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Quantity</t>
   </si>
@@ -86,15 +86,9 @@
     <t>369-1-010-0-NTX-KT0</t>
   </si>
   <si>
-    <t>Grid pitch: 1.27 mm BL2/15-0400GTT-010 RU MPE Garry Conten</t>
-  </si>
-  <si>
     <t>CN4</t>
   </si>
   <si>
-    <t>IEEE-488 IDC Connector Right Angle or Straight</t>
-  </si>
-  <si>
     <t>CN5</t>
   </si>
   <si>
@@ -246,6 +240,12 @@
   </si>
   <si>
     <t>I/O Controller Interface IC Versatile Interface Adapter</t>
+  </si>
+  <si>
+    <t>369-1-024-0-NTX-KT0</t>
+  </si>
+  <si>
+    <t>Female Header Micro Match 1,27 mm Wire to Board Connector Series 369</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,9 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -690,20 +692,24 @@
         <v>18</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="E6" s="4" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -711,16 +717,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -728,16 +734,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -745,16 +751,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -762,16 +768,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -779,16 +785,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -796,16 +802,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -813,16 +819,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -830,16 +836,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -847,16 +853,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -864,16 +870,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -881,16 +887,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -898,16 +904,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -915,16 +921,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -932,16 +938,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -949,16 +955,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All files updated to the latest version
</commit_message>
<xml_diff>
--- a/BOM/TriMod Adapter 2.xlsx
+++ b/BOM/TriMod Adapter 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\TriMod_2.0_Adapter\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elektronik\Altium\Projects\TriMod Adapter 2\Project Outputs for TriMod Adapter 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Quantity</t>
   </si>
@@ -86,9 +86,15 @@
     <t>369-1-010-0-NTX-KT0</t>
   </si>
   <si>
+    <t>Grid pitch: 1.27 mm BL2/15-0400GTT-010 RU MPE Garry Conten</t>
+  </si>
+  <si>
     <t>CN4</t>
   </si>
   <si>
+    <t>IEEE-488 IDC Connector Right Angle or Straight</t>
+  </si>
+  <si>
     <t>CN5</t>
   </si>
   <si>
@@ -240,12 +246,6 @@
   </si>
   <si>
     <t>I/O Controller Interface IC Versatile Interface Adapter</t>
-  </si>
-  <si>
-    <t>369-1-024-0-NTX-KT0</t>
-  </si>
-  <si>
-    <t>Female Header Micro Match 1,27 mm Wire to Board Connector Series 369</t>
   </si>
 </sst>
 </file>
@@ -599,9 +599,7 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -692,24 +690,20 @@
         <v>18</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -717,16 +711,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -734,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -751,16 +745,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -768,16 +762,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -785,16 +779,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -802,16 +796,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -819,16 +813,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -836,16 +830,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -853,16 +847,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -870,16 +864,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -887,16 +881,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -904,16 +898,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -921,16 +915,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -938,16 +932,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -955,16 +949,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>